<commit_message>
just backup - importing between files
</commit_message>
<xml_diff>
--- a/PDF-SaoKeNH/63000T9short_output.xlsx
+++ b/PDF-SaoKeNH/63000T9short_output.xlsx
@@ -18,6 +18,7 @@
     <sheet name="0008" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="0009" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="0010" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="00101" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2184,6 +2185,696 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ngày
+Date
+</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ghi chú
+Remark
+</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nợ
+Dr
+</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ccó
+Cr
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Số dư
+Balance
+</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Số tham chiếu
+Ref. no
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6502CALNNGOC
+MA_GD:106893563|K184131495,
+Hoe phi,
+HK01/2020-2021[201TO23@1@157
+HK01/2020-2021
+604000][BPMENT-DP-967482]
+</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 604,000
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 815,140,820
+</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> VBA
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6502CALNNGOC
+MA_GD:106893566|K184131495,
+Hoe phi,
+HK01/2020-2021[201TC18@99@16
+HK01/2020-2021
+906000][BPMENT-DP-967485]
+</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 906,000
+</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 816,046,820
+</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> VBA
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:106907741|K185021700,
+Hoc
+phiHK01,HK01,HK01,HK01,HKO1,I
+HK01/2020-2021
+50000][1653801@4@165380[ BPME
+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6,135,000
+</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 822,181,820
+</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 15/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA _GD:106964654|K184050616,
+Hoc
+phiHK01,HK01,HK01,HKO1,HKO1,I
+HK01/2020-2021
+50000][1654498@4@1654498@Phif
+</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5,833,000
+</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 828,014,820
+</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107043003|K184020190,
+Hoc
+phiHK01,HK01,HK01,HK01,HKO1,I
+HK01/2020-2021
+50000][1653685@4@1653685@Phif
+</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5,531,000
+</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 833,545,820
+</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107043427|K194081064,
+Hoc
+phiHK01,HK01,HK01,HKO1,HKO1,I
+HK01/2020-2021
+50000][1623154@4@162315[BPME
+</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5,531,000
+</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 839,076,820
+</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107054400|K194030292,
+Hoc
+phiHK01,HK01,HK01,HK01,HKO1,I
+HK01/2020-2021
+50000][1621762@4@1[BPMENT-F’
+</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 7,041,000
+</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 846,117,820
+</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107055538|K195011928,
+Hoc
+phiHK01,HK01,HK01,HKO1,HKO1,I
+HK01/2020-2021
+50000][1623280@4@1623280@Phit
+</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 10,875,000
+</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 856,992,820
+</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107060627|K194081104,
+Hoc
+phiHK01,HK01,HK01,HK01,HKO1,I
+HK01/2020-2021
+50000][1622543@4@162254[BPME
+</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5,531,000
+</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 862,523,820
+</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107063895|K174091025,
+Hoc
+phiHK01,HK01,HK01,HKO1,HKO1,I
+HK01/2020-2021
+50000][201KK28@1@1592053@Ke
+</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3,719,000
+</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 866,242,820
+</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 412803-Agribank; 1600201063000;N:
+Kim Hoang Quyen K184070930 nop
+Le phi phuc khao HKI18-19
+</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 50,000
+</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 866,292,820
+</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> VBA
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA _GD:107067056|K195042239,
+Hoc
+phiHK01,HK01,HK01,HKO1,HKO1,I
+HK01/2020-2021
+50000][1622236@4@162223[BPME
+</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6,437,000
+</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 872,729,820
+</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107076785|K194141756,
+Hoc
+phiHK05/2019-2020;HK01,HKO1,HI
+HK[BPMENT-FT-150846]
+</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12,301,000
+</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 885,030,820
+</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 16/09/2020
+</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> MA_GD:107082158|K194111578,
+Hoc
+phiHK01,HK01,HK01,HK0O1,HKO1,I
+HK01/2020-2021
+50000][201 DL06@1@1[BPMENT-F
+</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6,437,000
+</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 891,467,820
+</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>